<commit_message>
Fiche commandes git + MAJ Comptes
</commit_message>
<xml_diff>
--- a/Comptes_LaserTag.xlsx
+++ b/Comptes_LaserTag.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaftChoupi !\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10890" windowHeight="6750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10896" windowHeight="6756"/>
   </bookViews>
   <sheets>
     <sheet name="LaserTag" sheetId="2" r:id="rId1"/>
@@ -17,14 +12,14 @@
     <sheet name="_Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="USER">_Data!$A$2:$A$6</definedName>
+    <definedName name="USER">_Data!$A$2:$A$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
   <si>
     <t>Tableau pour le remboursement</t>
   </si>
@@ -161,9 +156,6 @@
     <t>Magasin</t>
   </si>
   <si>
-    <t>Liste des achats</t>
-  </si>
-  <si>
     <t>Dettes</t>
   </si>
   <si>
@@ -176,9 +168,6 @@
     <t>Total des dépenses</t>
   </si>
   <si>
-    <t>Remboursement par personnes</t>
-  </si>
-  <si>
     <t>Led émétrice (120) - RS</t>
   </si>
   <si>
@@ -194,13 +183,52 @@
     <t>Checksum</t>
   </si>
   <si>
-    <t>Frais de livraison (Moitié payée par Nabil, total 120€)</t>
-  </si>
-  <si>
     <t>Tubes PVC</t>
   </si>
   <si>
     <t>Lentilles (40) + plaques proto (20) - Aliexpress</t>
+  </si>
+  <si>
+    <t>Nbr Kit</t>
+  </si>
+  <si>
+    <t>pneu</t>
+  </si>
+  <si>
+    <t>flemme</t>
+  </si>
+  <si>
+    <t>emblask</t>
+  </si>
+  <si>
+    <t>Rbt / kit</t>
+  </si>
+  <si>
+    <t>Frais de livraison (autre moitié)</t>
+  </si>
+  <si>
+    <t>Liste des dépenses non-partagés</t>
+  </si>
+  <si>
+    <t>Frais de livraison (Moitié payée par flemme, total 120€)</t>
+  </si>
+  <si>
+    <t>Liste des dépenses partagés</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Dépenses</t>
+  </si>
+  <si>
+    <t>Supplément</t>
+  </si>
+  <si>
+    <t>Sup/Kit</t>
+  </si>
+  <si>
+    <t>Dépenses supplémentaires non-partagés</t>
   </si>
 </sst>
 </file>
@@ -212,7 +240,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1]"/>
     <numFmt numFmtId="165" formatCode="#,##0&quot;€&quot;"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -270,6 +298,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -292,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -361,20 +396,42 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="16">
     <dxf>
       <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -410,6 +467,103 @@
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -424,16 +578,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A11:F25" totalsRowShown="0">
-  <autoFilter ref="A11:F25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A16:F33" totalsRowShown="0">
+  <autoFilter ref="A16:F33"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Date" dataDxfId="6"/>
-    <tableColumn id="2" name="From" dataDxfId="5"/>
-    <tableColumn id="3" name="To" dataDxfId="4"/>
-    <tableColumn id="4" name="Libellé" dataDxfId="3"/>
-    <tableColumn id="5" name="Montant" dataDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="8" name="Remboursement par personnes" dataDxfId="1" dataCellStyle="Currency">
-      <calculatedColumnFormula>Table1[[#This Row],[Montant]]/4</calculatedColumnFormula>
+    <tableColumn id="1" name="Date" dataDxfId="8"/>
+    <tableColumn id="2" name="From" dataDxfId="7"/>
+    <tableColumn id="3" name="To" dataDxfId="6"/>
+    <tableColumn id="4" name="Libellé" dataDxfId="5"/>
+    <tableColumn id="5" name="Montant" dataDxfId="4"/>
+    <tableColumn id="8" name="Rbt / kit" dataDxfId="3">
+      <calculatedColumnFormula>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -441,13 +595,66 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:B8" totalsRowShown="0">
-  <autoFilter ref="A4:B8"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A10:C13" totalsRowShown="0">
+  <autoFilter ref="A10:C13"/>
+  <sortState ref="A12:C14">
+    <sortCondition descending="1" ref="A11:A14"/>
+  </sortState>
+  <tableColumns count="3">
     <tableColumn id="1" name="Nom"/>
-    <tableColumn id="2" name="Dettes" dataDxfId="0" dataCellStyle="Currency">
-      <calculatedColumnFormula>SUMIF(Table1[To],Table2[[#This Row],[Nom]],Table1[Montant])-SUMIF(Table1[From],Table2[[#This Row],[Nom]],Table1[Montant])+SUM(Table1[Remboursement par personnes])</calculatedColumnFormula>
+    <tableColumn id="2" name="Dettes" dataDxfId="14">
+      <calculatedColumnFormula>SUMIF(Table1[To],Table2[[#This Row],[Nom]],Table1[Montant])-SUMIF(Table1[From],Table2[[#This Row],[Nom]],Table1[Montant])+SUM(Table1[Rbt / kit])*Table2[[#This Row],[Nbr Kit]]</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="3" name="Nbr Kit" dataDxfId="15">
+      <calculatedColumnFormula>INDEX(Table26[],MATCH(Table2[[#This Row],[Nom]],Table26[Nom],0),MATCH(Table26[[#Headers],[Nbr Kit]],Table26[#Headers],0))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A44:E46" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A44:E46"/>
+  <sortState ref="A31:E36">
+    <sortCondition ref="A30:A36"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Date" dataDxfId="13"/>
+    <tableColumn id="2" name="From" dataDxfId="12"/>
+    <tableColumn id="3" name="To"/>
+    <tableColumn id="4" name="Libellé" dataDxfId="11"/>
+    <tableColumn id="5" name="Montant" dataDxfId="10" dataCellStyle="Monétaire"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A38:C41" totalsRowShown="0">
+  <autoFilter ref="A38:C41"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom"/>
+    <tableColumn id="2" name="Supplément" dataDxfId="0">
+      <calculatedColumnFormula>(-SUMIF(Tableau3[To],Table25[[#This Row],[Nom]],Tableau3[Montant])+SUMIF(Tableau3[From],Table25[[#This Row],[Nom]],Tableau3[Montant]))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Sup/Kit" dataCellStyle="Monétaire">
+      <calculatedColumnFormula>Table25[[#This Row],[Supplément]]/INDEX(Table26[],MATCH(Table25[[#This Row],[Nom]],Table26[Nom],0),MATCH(Table26[[#Headers],[Nbr Kit]],Table26[#Headers],0))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A4:C7" totalsRowShown="0">
+  <autoFilter ref="A4:C7"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Nom"/>
+    <tableColumn id="2" name="Dépenses" dataDxfId="1">
+      <calculatedColumnFormula>$F$15*Table26[Nbr Kit]+INDEX(Table25[],MATCH(Table26[[#This Row],[Nom]],Table25[Nom],0),MATCH(Table25[[#Headers],[Supplément]],Table25[#Headers],0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Nbr Kit" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -708,7 +915,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -716,499 +923,736 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="58.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="29">
-        <f>SUM(Table2[Dettes])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B5" s="11">
-        <f>SUMIF(Table1[To],Table2[[#This Row],[Nom]],Table1[Montant])-SUMIF(Table1[From],Table2[[#This Row],[Nom]],Table1[Montant])+SUM(Table1[Remboursement par personnes])</f>
-        <v>52.162499999999994</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <f>$F$15*Table26[Nbr Kit]+INDEX(Table25[],MATCH(Table26[[#This Row],[Nom]],Table25[Nom],0),MATCH(Table25[[#Headers],[Supplément]],Table25[#Headers],0))</f>
+        <v>120.79875</v>
+      </c>
+      <c r="C5" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B6" s="11">
-        <f>SUMIF(Table1[To],Table2[[#This Row],[Nom]],Table1[Montant])-SUMIF(Table1[From],Table2[[#This Row],[Nom]],Table1[Montant])+SUM(Table1[Remboursement par personnes])</f>
-        <v>75.532499999999999</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <f>$F$15*Table26[Nbr Kit]+INDEX(Table25[],MATCH(Table26[[#This Row],[Nom]],Table25[Nom],0),MATCH(Table25[[#Headers],[Supplément]],Table25[#Headers],0))</f>
+        <v>140.79874999999998</v>
+      </c>
+      <c r="C6" s="32">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B7" s="11">
-        <f>SUMIF(Table1[To],Table2[[#This Row],[Nom]],Table1[Montant])-SUMIF(Table1[From],Table2[[#This Row],[Nom]],Table1[Montant])+SUM(Table1[Remboursement par personnes])</f>
-        <v>-203.22749999999999</v>
-      </c>
-      <c r="C7" s="3"/>
+        <f>$F$15*Table26[Nbr Kit]+INDEX(Table25[],MATCH(Table26[[#This Row],[Nom]],Table25[Nom],0),MATCH(Table25[[#Headers],[Supplément]],Table25[#Headers],0))</f>
+        <v>80.532499999999999</v>
+      </c>
+      <c r="C7" s="32">
+        <v>2</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="11">
-        <f>SUMIF(Table1[To],Table2[[#This Row],[Nom]],Table1[Montant])-SUMIF(Table1[From],Table2[[#This Row],[Nom]],Table1[Montant])+SUM(Table1[Remboursement par personnes])</f>
-        <v>75.532499999999999</v>
-      </c>
-      <c r="C8" s="3"/>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11"/>
+      <c r="C8" s="32"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="29">
+        <f>SUM(Table2[Dettes])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="31">
-        <f>SUM(Table1[Montant])</f>
-        <v>302.13</v>
-      </c>
-      <c r="F10" s="31">
-        <f>SUM(Table1[Remboursement par personnes])</f>
-        <v>75.532499999999999</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
-        <v>42709</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="11">
+        <f>SUMIF(Table1[To],Table2[[#This Row],[Nom]],Table1[Montant])-SUMIF(Table1[From],Table2[[#This Row],[Nom]],Table1[Montant])+SUM(Table1[Rbt / kit])*Table2[[#This Row],[Nbr Kit]]</f>
+        <v>97.428749999999994</v>
+      </c>
+      <c r="C11" s="31">
+        <f>INDEX(Table26[],MATCH(Table2[[#This Row],[Nom]],Table26[Nom],0),MATCH(Table26[[#Headers],[Nbr Kit]],Table26[#Headers],0))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="18">
-        <v>23.37</v>
-      </c>
-      <c r="F12" s="18">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>5.8425000000000002</v>
+      <c r="B12" s="11">
+        <f>SUMIF(Table1[To],Table2[[#This Row],[Nom]],Table1[Montant])-SUMIF(Table1[From],Table2[[#This Row],[Nom]],Table1[Montant])+SUM(Table1[Rbt / kit])*Table2[[#This Row],[Nbr Kit]]</f>
+        <v>-177.96125000000001</v>
+      </c>
+      <c r="C12" s="31">
+        <f>INDEX(Table26[],MATCH(Table2[[#This Row],[Nom]],Table26[Nom],0),MATCH(Table26[[#Headers],[Nbr Kit]],Table26[#Headers],0))</f>
+        <v>3</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="11">
+        <f>SUMIF(Table1[To],Table2[[#This Row],[Nom]],Table1[Montant])-SUMIF(Table1[From],Table2[[#This Row],[Nom]],Table1[Montant])+SUM(Table1[Rbt / kit])*Table2[[#This Row],[Nbr Kit]]</f>
+        <v>80.532499999999999</v>
+      </c>
+      <c r="C13" s="31">
+        <f>INDEX(Table26[],MATCH(Table2[[#This Row],[Nom]],Table26[Nom],0),MATCH(Table26[[#Headers],[Nbr Kit]],Table26[#Headers],0))</f>
+        <v>2</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="37">
+        <f>SUM(Table1[Montant])</f>
+        <v>322.13</v>
+      </c>
+      <c r="F15" s="37">
+        <f>SUM(Table1[Rbt / kit])</f>
+        <v>40.266249999999999</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
         <v>42709</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="B17" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="19">
+      <c r="D17" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="18">
+        <v>23.37</v>
+      </c>
+      <c r="F17" s="18">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>2.9212500000000001</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>42709</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="19">
         <v>64.08</v>
       </c>
-      <c r="F13" s="19">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>16.02</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17">
+      <c r="F18" s="19">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>8.01</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
         <v>42709</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="B19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="19">
+      <c r="D19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="19">
         <v>82.88</v>
       </c>
-      <c r="F14" s="21">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>20.72</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17">
+      <c r="F19" s="21">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>10.36</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
         <v>42709</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="15" t="s">
+      <c r="B20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="19">
-        <v>0</v>
-      </c>
-      <c r="F15" s="21">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="17">
-        <v>42712</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="19">
-        <v>51.8</v>
-      </c>
-      <c r="F16" s="21">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>12.95</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17">
-        <v>42730</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="19">
-        <v>80</v>
-      </c>
-      <c r="F17" s="21">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>20</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
-      <c r="B18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="24">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="24">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="23"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="24">
-        <f>Table1[[#This Row],[Montant]]/4</f>
+      <c r="D20" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="19">
+        <v>0</v>
+      </c>
+      <c r="F20" s="21">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
         <v>0</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="24">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>0</v>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>42712</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="19">
+        <v>51.8</v>
+      </c>
+      <c r="F21" s="21">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>6.4749999999999996</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="27">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>0</v>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>42730</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="19">
+        <v>100</v>
+      </c>
+      <c r="F22" s="21">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>12.5</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="25"/>
+      <c r="B23" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="E23" s="21"/>
-      <c r="F23" s="27">
-        <f>Table1[[#This Row],[Montant]]/4</f>
+      <c r="F23" s="24">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
         <v>0</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
-      <c r="D24" s="25"/>
+      <c r="D24" s="14"/>
       <c r="E24" s="21"/>
-      <c r="F24" s="27">
-        <f>Table1[[#This Row],[Montant]]/4</f>
+      <c r="F24" s="24">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
         <v>0</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="27">
-        <f>Table1[[#This Row],[Montant]]/4</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F27" s="2"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="24">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="24">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="27">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="27">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D29" s="5"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="I28" s="3"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="27">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="4"/>
+      <c r="I29" s="3"/>
       <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E30" s="4"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B35" s="2"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="27">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="35">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="35">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="35">
+        <f>Table1[[#This Row],[Montant]]/SUM(Table2[Nbr Kit])</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="11">
+        <f>(-SUMIF(Tableau3[To],Table25[[#This Row],[Nom]],Tableau3[Montant])+SUMIF(Tableau3[From],Table25[[#This Row],[Nom]],Tableau3[Montant]))</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="38">
+        <f>Table25[[#This Row],[Supplément]]/INDEX(Table26[],MATCH(Table25[[#This Row],[Nom]],Table26[Nom],0),MATCH(Table26[[#Headers],[Nbr Kit]],Table26[#Headers],0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="11">
+        <f>(-SUMIF(Tableau3[To],Table25[[#This Row],[Nom]],Tableau3[Montant])+SUMIF(Tableau3[From],Table25[[#This Row],[Nom]],Tableau3[Montant]))</f>
+        <v>20</v>
+      </c>
+      <c r="C40" s="39">
+        <f>Table25[[#This Row],[Supplément]]/INDEX(Table26[],MATCH(Table25[[#This Row],[Nom]],Table26[Nom],0),MATCH(Table26[[#Headers],[Nbr Kit]],Table26[#Headers],0))</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="11">
+        <f>(-SUMIF(Tableau3[To],Table25[[#This Row],[Nom]],Tableau3[Montant])+SUMIF(Tableau3[From],Table25[[#This Row],[Nom]],Tableau3[Montant]))</f>
+        <v>0</v>
+      </c>
+      <c r="C41" s="39">
+        <f>Table25[[#This Row],[Supplément]]/INDEX(Table26[],MATCH(Table25[[#This Row],[Nom]],Table26[Nom],0),MATCH(Table26[[#Headers],[Nbr Kit]],Table26[#Headers],0))</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="D42" s="5"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="37">
+        <f>SUM(Tableau3[Montant])</f>
+        <v>20</v>
+      </c>
+      <c r="F43" s="30"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="17">
+        <v>42730</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" s="19">
+        <v>20</v>
+      </c>
+      <c r="F45" s="18"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="K45" s="4"/>
+    </row>
+    <row r="46" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="16"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="19"/>
+    </row>
+    <row r="47" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="17"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="21"/>
+    </row>
+    <row r="48" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A48" s="17"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="21"/>
+    </row>
+    <row r="49" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A49" s="17"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="21"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="17"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="21"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:C25 A5:A8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:C46 A11:A13 B17:C35 A39:A41 A5:A8">
       <formula1>USER</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1221,29 +1665,29 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1275,7 +1719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1304,7 +1748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1333,7 +1777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1362,7 +1806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1379,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1408,7 +1852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1431,7 +1875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1454,7 +1898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="4">
         <f>SUM(C7:C13)</f>
         <v>150.47</v>
@@ -1487,7 +1931,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="3">
         <f t="shared" ref="E15:J15" si="1">E8*$C8/SUM($E8:$J8)</f>
         <v>6.25</v>
@@ -1513,7 +1957,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="3">
         <f t="shared" ref="E16:J16" si="2">E9*$C9/SUM($E9:$J9)</f>
         <v>6.75</v>
@@ -1539,7 +1983,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E17" s="3">
         <f t="shared" ref="E17:J17" si="3">E10*$C10/SUM($E10:$J10)</f>
         <v>0</v>
@@ -1565,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E18" s="3">
         <f t="shared" ref="E18:J18" si="4">E11*$C11/SUM($E11:$J11)</f>
         <v>3.75</v>
@@ -1591,7 +2035,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="3">
         <f t="shared" ref="E19:J19" si="5">E12*$C12/SUM($E12:$J12)</f>
         <v>8.5879999999999992</v>
@@ -1617,7 +2061,7 @@
         <v>4.2939999999999996</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="3">
         <f t="shared" ref="E20:J20" si="6">E13*$C13/SUM($E13:$J13)</f>
         <v>8</v>
@@ -1646,7 +2090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="5" t="s">
         <v>22</v>
       </c>
@@ -1679,7 +2123,7 @@
         <v>150.47</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="5" t="s">
         <v>23</v>
       </c>
@@ -1712,7 +2156,7 @@
         <v>150.47</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="5"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
@@ -1728,7 +2172,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="6" t="s">
         <v>25</v>
       </c>
@@ -1757,7 +2201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="6" t="s">
         <v>27</v>
       </c>
@@ -1793,7 +2237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F26" s="2" t="s">
         <v>28</v>
       </c>
@@ -1801,7 +2245,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D27" s="5"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1813,7 +2257,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D28" s="5" t="s">
         <v>30</v>
       </c>
@@ -1831,7 +2275,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E29" s="4"/>
       <c r="F29" s="3">
         <f>-J29</f>
@@ -1846,7 +2290,7 @@
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E30" s="3">
         <f>E25</f>
         <v>12.088000000000001</v>
@@ -1866,7 +2310,7 @@
       </c>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="D31" s="2" t="s">
         <v>31</v>
@@ -1900,15 +2344,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>33</v>
       </c>
@@ -1922,7 +2366,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
@@ -1937,41 +2381,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>